<commit_message>
Added check for if case statute or degree is none.
</commit_message>
<xml_diff>
--- a/db/Arraignments.xlsx
+++ b/db/Arraignments.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="109">
   <si>
     <t>Case</t>
   </si>
@@ -149,9 +149,6 @@
   </si>
   <si>
     <t>TURN AND STOP SIGNALS</t>
-  </si>
-  <si>
-    <t>4511.39</t>
   </si>
   <si>
     <t>21TRC08418-A</t>
@@ -788,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -821,7 +818,7 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.5">
@@ -847,7 +844,7 @@
         <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="38" x14ac:dyDescent="0.5">
@@ -873,7 +870,7 @@
         <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
@@ -899,7 +896,7 @@
         <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
@@ -925,7 +922,7 @@
         <v>30</v>
       </c>
       <c r="H5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
@@ -947,11 +944,9 @@
       <c r="F6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="G6" s="1"/>
       <c r="H6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="38" x14ac:dyDescent="0.5">
@@ -977,7 +972,7 @@
         <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
@@ -996,14 +991,12 @@
       <c r="E8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
@@ -1011,7 +1004,7 @@
         <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>39</v>
@@ -1020,212 +1013,212 @@
         <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="H9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="H11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="G13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="E14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="H14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="G15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>11</v>
@@ -1237,163 +1230,163 @@
         <v>13</v>
       </c>
       <c r="H17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="E21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="G21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
New DB connection working.
</commit_message>
<xml_diff>
--- a/db/Arraignments.xlsx
+++ b/db/Arraignments.xlsx
@@ -94,12 +94,6 @@
     <t>21CRB01268-A</t>
   </si>
   <si>
-    <t>DEAN</t>
-  </si>
-  <si>
-    <t>TARA</t>
-  </si>
-  <si>
     <t>POSSESSION DRUG PARAPHERNALIA</t>
   </si>
   <si>
@@ -341,6 +335,12 @@
   </si>
   <si>
     <t>U</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>TESET</t>
   </si>
 </sst>
 </file>
@@ -786,7 +786,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -818,7 +818,7 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.5">
@@ -844,7 +844,7 @@
         <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="38" x14ac:dyDescent="0.5">
@@ -870,7 +870,7 @@
         <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
@@ -896,7 +896,7 @@
         <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
@@ -907,318 +907,318 @@
         <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="H5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="H9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="H11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="G13" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="E14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="H14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="D15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="G15" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="D16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>11</v>
@@ -1230,163 +1230,163 @@
         <v>13</v>
       </c>
       <c r="H17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="D18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="D19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="D20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="E21" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="D22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="G22" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="D23" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H23" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
Working but using variables in query is not.
</commit_message>
<xml_diff>
--- a/db/Arraignments.xlsx
+++ b/db/Arraignments.xlsx
@@ -163,12 +163,6 @@
     <t>21CRB01437-A</t>
   </si>
   <si>
-    <t>MANCHESTER</t>
-  </si>
-  <si>
-    <t>LINDSEY</t>
-  </si>
-  <si>
     <t>POSSESSION OF MARIHUANA</t>
   </si>
   <si>
@@ -214,12 +208,6 @@
     <t>21CRB01387-A</t>
   </si>
   <si>
-    <t>MURPHY</t>
-  </si>
-  <si>
-    <t>KEVIN</t>
-  </si>
-  <si>
     <t>SEXUAL IMPOSITION M1</t>
   </si>
   <si>
@@ -341,6 +329,18 @@
   </si>
   <si>
     <t>TESET</t>
+  </si>
+  <si>
+    <t>KUDELA</t>
+  </si>
+  <si>
+    <t>JUSTIN</t>
+  </si>
+  <si>
+    <t>NETTLER</t>
+  </si>
+  <si>
+    <t>KATHERINE</t>
   </si>
 </sst>
 </file>
@@ -785,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -818,7 +818,7 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.5">
@@ -844,7 +844,7 @@
         <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="38" x14ac:dyDescent="0.5">
@@ -870,7 +870,7 @@
         <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
@@ -896,7 +896,7 @@
         <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
@@ -907,10 +907,10 @@
         <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>26</v>
@@ -922,7 +922,7 @@
         <v>28</v>
       </c>
       <c r="H5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
@@ -946,7 +946,7 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="38" x14ac:dyDescent="0.5">
@@ -972,7 +972,7 @@
         <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
@@ -996,7 +996,7 @@
         <v>17</v>
       </c>
       <c r="H8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
@@ -1022,7 +1022,7 @@
         <v>46</v>
       </c>
       <c r="H9" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="38" x14ac:dyDescent="0.5">
@@ -1033,114 +1033,114 @@
         <v>48</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H10" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="H11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H12" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>46</v>
       </c>
       <c r="H13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>44</v>
@@ -1152,73 +1152,73 @@
         <v>46</v>
       </c>
       <c r="H14" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="C15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>46</v>
       </c>
       <c r="H15" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H16" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>11</v>
@@ -1230,163 +1230,163 @@
         <v>13</v>
       </c>
       <c r="H17" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="C18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H18" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H19" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H20" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>46</v>
       </c>
       <c r="H21" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="C22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>28</v>
       </c>
       <c r="H22" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H23" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
Refactoring out query strings.
</commit_message>
<xml_diff>
--- a/db/Arraignments.xlsx
+++ b/db/Arraignments.xlsx
@@ -325,12 +325,6 @@
     <t>U</t>
   </si>
   <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>TESET</t>
-  </si>
-  <si>
     <t>KUDELA</t>
   </si>
   <si>
@@ -341,6 +335,12 @@
   </si>
   <si>
     <t>KATHERINE</t>
+  </si>
+  <si>
+    <t>DOUGLAS</t>
+  </si>
+  <si>
+    <t>MICHAEL</t>
   </si>
 </sst>
 </file>
@@ -786,7 +786,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -907,10 +907,10 @@
         <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>26</v>
@@ -1033,10 +1033,10 @@
         <v>48</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>49</v>
@@ -1111,10 +1111,10 @@
         <v>63</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
Updated CMS_FRALoader to set to N/A for CRB cases.
</commit_message>
<xml_diff>
--- a/db/Arraignments.xlsx
+++ b/db/Arraignments.xlsx
@@ -786,7 +786,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1048,7 +1048,7 @@
         <v>17</v>
       </c>
       <c r="H10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
Fixed costs for cost calculator.
</commit_message>
<xml_diff>
--- a/db/Arraignments.xlsx
+++ b/db/Arraignments.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="113">
   <si>
     <t>Case</t>
   </si>
@@ -341,6 +341,18 @@
   </si>
   <si>
     <t>MICHAEL</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Moving</t>
+  </si>
+  <si>
+    <t>Non-moving</t>
+  </si>
+  <si>
+    <t>Criminal</t>
   </si>
 </sst>
 </file>
@@ -783,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -795,7 +807,7 @@
     <col min="8" max="8" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -820,8 +832,11 @@
       <c r="H1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="I1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -846,8 +861,11 @@
       <c r="H2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="38" x14ac:dyDescent="0.5">
+      <c r="I2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="38" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -872,8 +890,11 @@
       <c r="H3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
+      <c r="I3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -898,8 +919,11 @@
       <c r="H4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
+      <c r="I4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -924,8 +948,11 @@
       <c r="H5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
+      <c r="I5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -948,8 +975,11 @@
       <c r="H6" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="38" x14ac:dyDescent="0.5">
+      <c r="I6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="38" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -974,8 +1004,11 @@
       <c r="H7" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
+      <c r="I7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
@@ -998,8 +1031,11 @@
       <c r="H8" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
+      <c r="I8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -1024,8 +1060,11 @@
       <c r="H9" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="38" x14ac:dyDescent="0.5">
+      <c r="I9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="38" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
@@ -1050,8 +1089,11 @@
       <c r="H10" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
+      <c r="I10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>51</v>
       </c>
@@ -1076,8 +1118,11 @@
       <c r="H11" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
+      <c r="I11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
@@ -1102,8 +1147,11 @@
       <c r="H12" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="38" x14ac:dyDescent="0.5">
+      <c r="I12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="38" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>62</v>
       </c>
@@ -1128,8 +1176,11 @@
       <c r="H13" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
+      <c r="I13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>66</v>
       </c>
@@ -1154,8 +1205,11 @@
       <c r="H14" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="I14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>66</v>
       </c>
@@ -1180,8 +1234,11 @@
       <c r="H15" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
+      <c r="I15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>66</v>
       </c>
@@ -1206,8 +1263,11 @@
       <c r="H16" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="I16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>76</v>
       </c>
@@ -1232,8 +1292,11 @@
       <c r="H17" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="38" x14ac:dyDescent="0.5">
+      <c r="I17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="38" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>76</v>
       </c>
@@ -1258,8 +1321,11 @@
       <c r="H18" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
+      <c r="I18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
         <v>76</v>
       </c>
@@ -1284,8 +1350,11 @@
       <c r="H19" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
+      <c r="I19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
         <v>76</v>
       </c>
@@ -1310,8 +1379,11 @@
       <c r="H20" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="I20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
         <v>89</v>
       </c>
@@ -1336,8 +1408,11 @@
       <c r="H21" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="38" x14ac:dyDescent="0.5">
+      <c r="I21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="38" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>89</v>
       </c>
@@ -1362,8 +1437,11 @@
       <c r="H22" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="38" x14ac:dyDescent="0.5">
+      <c r="I22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="38" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
         <v>89</v>
       </c>
@@ -1388,8 +1466,11 @@
       <c r="H23" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.5"/>
+      <c r="I23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="23.45" customHeight="1" x14ac:dyDescent="0.5"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="1" footer="1"/>

</xml_diff>

<commit_message>
Added Reload button - reloads deleted and added cases.
Button added test failing.


Button working to load but have duplicates.


Tests working for all daily cases lists delete and reload.


Reload working for adding cases to Excel reports.


Moved reload button to other side of UI.
</commit_message>
<xml_diff>
--- a/db/Arraignments.xlsx
+++ b/db/Arraignments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\AppData\Local\Programs\Python\Python310\MuniEntry\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCECCFE-C368-4589-96C8-5F3E26CC8847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9575EC50-250D-4D4A-A031-2DA64840814F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="9015" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27030" yWindow="10785" windowWidth="21600" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MuniEntryArraignment" sheetId="1" r:id="rId1"/>
@@ -781,7 +781,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
Cleaned some offenses for caps and OMVI to OVI.
</commit_message>
<xml_diff>
--- a/db/Arraignments.xlsx
+++ b/db/Arraignments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\AppData\Local\Programs\Python\Python310\MuniEntry\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9575EC50-250D-4D4A-A031-2DA64840814F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292A8BBF-916C-4C39-A9E7-C4AA05A3E41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27030" yWindow="10785" windowWidth="21600" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="9015" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MuniEntryArraignment" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="96">
   <si>
     <t>Case</t>
   </si>
@@ -160,9 +160,6 @@
     <t>22TRC02035-B</t>
   </si>
   <si>
-    <t>OVI BREATH 1ST .17 &amp; ABOVE</t>
-  </si>
-  <si>
     <t>4511.19A1H*</t>
   </si>
   <si>
@@ -305,6 +302,12 @@
   </si>
   <si>
     <t>22TRD01944-B</t>
+  </si>
+  <si>
+    <t>OVI BREATH 1ST .17 &amp; ABOVE M2</t>
+  </si>
+  <si>
+    <t>OMVI ALCOHOL / DRUGS 1ST M1</t>
   </si>
 </sst>
 </file>
@@ -781,7 +784,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1015,7 +1018,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" ht="25.5">
+    <row r="8" spans="1:12" ht="51">
       <c r="A8" s="1" t="s">
         <v>38</v>
       </c>
@@ -1029,7 +1032,7 @@
         <v>41</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>26</v>
@@ -1065,10 +1068,10 @@
         <v>41</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>27</v>
@@ -1088,7 +1091,7 @@
         <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>40</v>
@@ -1097,10 +1100,10 @@
         <v>41</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>35</v>
@@ -1117,16 +1120,16 @@
     </row>
     <row r="11" spans="1:12" ht="25.5">
       <c r="A11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>25</v>
@@ -1138,7 +1141,7 @@
         <v>27</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I11" s="2" t="b">
         <v>1</v>
@@ -1149,28 +1152,28 @@
     </row>
     <row r="12" spans="1:12" ht="38.25">
       <c r="A12" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="E12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>35</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I12" s="2" t="b">
         <v>1</v>
@@ -1181,19 +1184,19 @@
     </row>
     <row r="13" spans="1:12" ht="51">
       <c r="A13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>30</v>
@@ -1202,7 +1205,7 @@
         <v>31</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I13" s="2" t="b">
         <v>1</v>
@@ -1213,19 +1216,19 @@
     </row>
     <row r="14" spans="1:12" ht="38.25">
       <c r="A14" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>34</v>
@@ -1234,7 +1237,7 @@
         <v>31</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I14" s="2" t="b">
         <v>1</v>
@@ -1245,28 +1248,28 @@
     </row>
     <row r="15" spans="1:12" ht="51">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>35</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I15" s="2" t="b">
         <v>1</v>
@@ -1277,28 +1280,28 @@
     </row>
     <row r="16" spans="1:12" ht="25.5">
       <c r="A16" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="H16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I16" s="2" t="b">
         <v>1</v>
@@ -1309,19 +1312,19 @@
     </row>
     <row r="17" spans="1:12" ht="76.5">
       <c r="A17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>30</v>
@@ -1330,7 +1333,7 @@
         <v>31</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I17" s="2" t="b">
         <v>1</v>
@@ -1341,28 +1344,28 @@
     </row>
     <row r="18" spans="1:12" ht="51">
       <c r="A18" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>35</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I18" s="2" t="b">
         <v>1</v>
@@ -1373,22 +1376,22 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>31</v>
@@ -1405,22 +1408,22 @@
     </row>
     <row r="20" spans="1:12" ht="51">
       <c r="A20" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>35</v>
@@ -1437,28 +1440,28 @@
     </row>
     <row r="21" spans="1:12" ht="51">
       <c r="A21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I21" s="2" t="b">
         <v>1</v>
@@ -1469,16 +1472,16 @@
     </row>
     <row r="22" spans="1:12" ht="25.5">
       <c r="A22" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>33</v>
@@ -1490,7 +1493,7 @@
         <v>31</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I22" s="2" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Added Petty to delete word for clean offense list.
</commit_message>
<xml_diff>
--- a/db/Arraignments.xlsx
+++ b/db/Arraignments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\AppData\Local\Programs\Python\Python310\MuniEntry\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292A8BBF-916C-4C39-A9E7-C4AA05A3E41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E69BB2-2E58-4703-A02B-C11387F19F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="9015" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45972" yWindow="6996" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MuniEntryArraignment" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="97">
   <si>
     <t>Case</t>
   </si>
@@ -308,6 +308,9 @@
   </si>
   <si>
     <t>OMVI ALCOHOL / DRUGS 1ST M1</t>
+  </si>
+  <si>
+    <t>PETTY THEFT</t>
   </si>
 </sst>
 </file>
@@ -784,7 +787,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -875,7 +878,9 @@
       <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="F3" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Tests added for excel loader and allied and dismissed on charges grid.
Added test for column count check.


Added test for create_headers_dict


Updated path for excel tests.


Added tests for allied and dismissed and deleted attribute check decor
</commit_message>
<xml_diff>
--- a/db/Arraignments.xlsx
+++ b/db/Arraignments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\AppData\Local\Programs\Python\Python310\MuniEntry\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F75F8F4-8855-453C-B472-F4716C8D0661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9EFBD48-2182-4ABC-B835-24B536A26FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="9015" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -784,7 +784,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H7"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
Updated headers in case excel loaders and in db files.
</commit_message>
<xml_diff>
--- a/db/Arraignments.xlsx
+++ b/db/Arraignments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\AppData\Local\Programs\Python\Python310\MuniEntry\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkudela\AppData\Local\Programs\Python\Python310\MuniEntry\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9EFBD48-2182-4ABC-B835-24B536A26FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8311F8B8-0ACF-4555-B057-45ABE4BC26F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="9015" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MuniEntryArraignment" sheetId="1" r:id="rId1"/>
@@ -20,43 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="96">
-  <si>
-    <t>Case</t>
-  </si>
-  <si>
-    <t>Sub Case</t>
-  </si>
-  <si>
-    <t>Lastname</t>
-  </si>
-  <si>
-    <t>Firstname</t>
-  </si>
-  <si>
-    <t>Charge</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Degree</t>
-  </si>
-  <si>
-    <t>Insurance</t>
-  </si>
-  <si>
-    <t>Moving</t>
-  </si>
-  <si>
-    <t>Atty Last</t>
-  </si>
-  <si>
-    <t>Atty First</t>
-  </si>
-  <si>
-    <t>Atty Type</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="97">
   <si>
     <t>22CRB00236</t>
   </si>
@@ -308,6 +272,45 @@
   </si>
   <si>
     <t>O'METZ</t>
+  </si>
+  <si>
+    <t>DefFirstName</t>
+  </si>
+  <si>
+    <t>CaseNumber</t>
+  </si>
+  <si>
+    <t>SubCaseNumber</t>
+  </si>
+  <si>
+    <t>DefLastName</t>
+  </si>
+  <si>
+    <t>ChargeDescription</t>
+  </si>
+  <si>
+    <t>SectionCode</t>
+  </si>
+  <si>
+    <t>DegreeCode</t>
+  </si>
+  <si>
+    <t>InsuranceStatus</t>
+  </si>
+  <si>
+    <t>IsMoving</t>
+  </si>
+  <si>
+    <t>AttorneyLastName</t>
+  </si>
+  <si>
+    <t>AttorneyFirstName</t>
+  </si>
+  <si>
+    <t>PubDef</t>
+  </si>
+  <si>
+    <t>U</t>
   </si>
 </sst>
 </file>
@@ -783,716 +786,763 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="12" width="13.73046875" customWidth="1"/>
+    <col min="1" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" ht="25.5">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>87</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>90</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>92</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>93</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>94</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="63.75">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="2" t="b">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I2" s="2">
         <v>0</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="25.5">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="2" t="b">
+      <c r="I3" s="2">
         <v>0</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="25.5">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="2" t="b">
+      <c r="I4" s="2">
         <v>1</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" ht="38.25">
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="51">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="2" t="b">
+      <c r="I5" s="2">
         <v>1</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="25.5">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="2" t="b">
+      <c r="I6" s="2">
         <v>1</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="25.5">
       <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="2" t="b">
+      <c r="I7" s="2">
         <v>1</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="L7" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="51">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" s="2" t="b">
+        <v>29</v>
+      </c>
+      <c r="I8" s="2">
         <v>1</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L8" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="38.25">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" s="2" t="b">
+        <v>29</v>
+      </c>
+      <c r="I9" s="2">
         <v>1</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="38.25">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I10" s="2" t="b">
+        <v>29</v>
+      </c>
+      <c r="I10" s="2">
         <v>1</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
+      <c r="L10" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="25.5">
       <c r="A11" s="1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I11" s="2" t="b">
+        <v>41</v>
+      </c>
+      <c r="I11" s="2">
         <v>1</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="L11" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="38.25">
       <c r="A12" s="1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I12" s="2" t="b">
+        <v>41</v>
+      </c>
+      <c r="I12" s="2">
         <v>1</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
+      <c r="L12" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="51">
       <c r="A13" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I13" s="2" t="b">
+        <v>41</v>
+      </c>
+      <c r="I13" s="2">
         <v>1</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:12" ht="38.25">
       <c r="A14" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I14" s="2" t="b">
+        <v>41</v>
+      </c>
+      <c r="I14" s="2">
         <v>1</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
+      <c r="L14" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="51">
       <c r="A15" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I15" s="2" t="b">
+        <v>41</v>
+      </c>
+      <c r="I15" s="2">
         <v>1</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
+      <c r="L15" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:12" ht="25.5">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="G16" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I16" s="2" t="b">
+        <v>41</v>
+      </c>
+      <c r="I16" s="2">
         <v>1</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
+      <c r="L16" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:12" ht="76.5">
       <c r="A17" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I17" s="2" t="b">
+        <v>41</v>
+      </c>
+      <c r="I17" s="2">
         <v>1</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
+      <c r="L17" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:12" ht="51">
       <c r="A18" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I18" s="2" t="b">
+        <v>41</v>
+      </c>
+      <c r="I18" s="2">
         <v>1</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+      <c r="L18" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I19" s="2" t="b">
+        <v>29</v>
+      </c>
+      <c r="I19" s="2">
         <v>1</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
+      <c r="L19" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:12" ht="51">
       <c r="A20" s="1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I20" s="2" t="b">
+        <v>29</v>
+      </c>
+      <c r="I20" s="2">
         <v>1</v>
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
+      <c r="L20" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:12" ht="51">
       <c r="A21" s="1" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I21" s="2" t="b">
+        <v>41</v>
+      </c>
+      <c r="I21" s="2">
         <v>1</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
+      <c r="L21" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:12" ht="25.5">
       <c r="A22" s="1" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I22" s="2" t="b">
+        <v>41</v>
+      </c>
+      <c r="I22" s="2">
         <v>1</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-    </row>
-    <row r="23" spans="1:12" ht="23.55" customHeight="1"/>
+      <c r="L22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="23.65" customHeight="1"/>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="1" footer="1"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Fixed hyphenated last name with space issue.
</commit_message>
<xml_diff>
--- a/db/Arraignments.xlsx
+++ b/db/Arraignments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkudela\AppData\Local\Programs\Python\Python310\MuniEntry\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8311F8B8-0ACF-4555-B057-45ABE4BC26F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF99B472-F019-4AB7-9466-332D34C8C801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MuniEntryArraignment" sheetId="1" r:id="rId1"/>
@@ -139,9 +139,6 @@
     <t>22TRC02124-A</t>
   </si>
   <si>
-    <t>Smith</t>
-  </si>
-  <si>
     <t>Joey</t>
   </si>
   <si>
@@ -311,6 +308,9 @@
   </si>
   <si>
     <t>U</t>
+  </si>
+  <si>
+    <t>Smith - Jones</t>
   </si>
 </sst>
 </file>
@@ -786,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -800,40 +800,40 @@
   <sheetData>
     <row r="1" spans="1:12" ht="25.5">
       <c r="A1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="63.75">
@@ -859,7 +859,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I2" s="2">
         <v>0</v>
@@ -884,7 +884,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>5</v>
@@ -1042,7 +1042,7 @@
         <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>13</v>
@@ -1080,7 +1080,7 @@
         <v>27</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>33</v>
@@ -1136,7 +1136,7 @@
     </row>
     <row r="11" spans="1:12" ht="25.5">
       <c r="A11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>37</v>
@@ -1145,7 +1145,7 @@
         <v>38</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>39</v>
+        <v>96</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>12</v>
@@ -1157,7 +1157,7 @@
         <v>14</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I11" s="2">
         <v>1</v>
@@ -1170,16 +1170,16 @@
     </row>
     <row r="12" spans="1:12" ht="38.25">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>39</v>
+        <v>96</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>35</v>
@@ -1191,7 +1191,7 @@
         <v>22</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I12" s="2">
         <v>1</v>
@@ -1204,19 +1204,19 @@
     </row>
     <row r="13" spans="1:12" ht="51">
       <c r="A13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>17</v>
@@ -1225,7 +1225,7 @@
         <v>18</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I13" s="2">
         <v>1</v>
@@ -1238,19 +1238,19 @@
     </row>
     <row r="14" spans="1:12" ht="38.25">
       <c r="A14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>21</v>
@@ -1259,7 +1259,7 @@
         <v>18</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I14" s="2">
         <v>1</v>
@@ -1272,28 +1272,28 @@
     </row>
     <row r="15" spans="1:12" ht="51">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I15" s="2">
         <v>1</v>
@@ -1306,28 +1306,28 @@
     </row>
     <row r="16" spans="1:12" ht="25.5">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="H16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I16" s="2">
         <v>1</v>
@@ -1340,19 +1340,19 @@
     </row>
     <row r="17" spans="1:12" ht="76.5">
       <c r="A17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>17</v>
@@ -1361,7 +1361,7 @@
         <v>18</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I17" s="2">
         <v>1</v>
@@ -1374,28 +1374,28 @@
     </row>
     <row r="18" spans="1:12" ht="51">
       <c r="A18" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I18" s="2">
         <v>1</v>
@@ -1408,22 +1408,22 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>18</v>
@@ -1442,22 +1442,22 @@
     </row>
     <row r="20" spans="1:12" ht="51">
       <c r="A20" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>22</v>
@@ -1476,28 +1476,28 @@
     </row>
     <row r="21" spans="1:12" ht="51">
       <c r="A21" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I21" s="2">
         <v>1</v>
@@ -1510,16 +1510,16 @@
     </row>
     <row r="22" spans="1:12" ht="25.5">
       <c r="A22" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>20</v>
@@ -1531,7 +1531,7 @@
         <v>18</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I22" s="2">
         <v>1</v>

</xml_diff>